<commit_message>
Comparision simulations for extended batch are ongoing
</commit_message>
<xml_diff>
--- a/experiments/pg/range_m10_10_compare_mlp_1_hidden/start_3_m3_3_max_step_1_traj_60_batch_200_shared_1x256_sep_1_step_3e_3_alpha_ret_1e_1_ext_batch_alpha_1e_p1/oracle_buffer.xlsx
+++ b/experiments/pg/range_m10_10_compare_mlp_1_hidden/start_3_m3_3_max_step_1_traj_60_batch_200_shared_1x256_sep_1_step_3e_3_alpha_ret_1e_1_ext_batch_alpha_1e_p1/oracle_buffer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4842"/>
+  <dimension ref="A1:C4873"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -63378,6 +63378,409 @@
         <v>13.91166398113202</v>
       </c>
     </row>
+    <row r="4843">
+      <c r="A4843" s="1" t="n">
+        <v>4841</v>
+      </c>
+      <c r="B4843" t="inlineStr">
+        <is>
+          <t>[6, 5, -6]</t>
+        </is>
+      </c>
+      <c r="C4843" t="n">
+        <v>14.03652477627304</v>
+      </c>
+    </row>
+    <row r="4844">
+      <c r="A4844" s="1" t="n">
+        <v>4842</v>
+      </c>
+      <c r="B4844" t="inlineStr">
+        <is>
+          <t>[7, 5, -6]</t>
+        </is>
+      </c>
+      <c r="C4844" t="n">
+        <v>14.01631281144186</v>
+      </c>
+    </row>
+    <row r="4845">
+      <c r="A4845" s="1" t="n">
+        <v>4843</v>
+      </c>
+      <c r="B4845" t="inlineStr">
+        <is>
+          <t>[8, 5, -6]</t>
+        </is>
+      </c>
+      <c r="C4845" t="n">
+        <v>13.94895842817975</v>
+      </c>
+    </row>
+    <row r="4846">
+      <c r="A4846" s="1" t="n">
+        <v>4844</v>
+      </c>
+      <c r="B4846" t="inlineStr">
+        <is>
+          <t>[8, 2, -2]</t>
+        </is>
+      </c>
+      <c r="C4846" t="n">
+        <v>14.09184525911637</v>
+      </c>
+    </row>
+    <row r="4847">
+      <c r="A4847" s="1" t="n">
+        <v>4845</v>
+      </c>
+      <c r="B4847" t="inlineStr">
+        <is>
+          <t>[10, 6, -8]</t>
+        </is>
+      </c>
+      <c r="C4847" t="n">
+        <v>13.91210366446522</v>
+      </c>
+    </row>
+    <row r="4848">
+      <c r="A4848" s="1" t="n">
+        <v>4846</v>
+      </c>
+      <c r="B4848" t="inlineStr">
+        <is>
+          <t>[3, 7, -10]</t>
+        </is>
+      </c>
+      <c r="C4848" t="n">
+        <v>14.20976903201439</v>
+      </c>
+    </row>
+    <row r="4849">
+      <c r="A4849" s="1" t="n">
+        <v>4847</v>
+      </c>
+      <c r="B4849" t="inlineStr">
+        <is>
+          <t>[6, 7, -10]</t>
+        </is>
+      </c>
+      <c r="C4849" t="n">
+        <v>14.0077136202595</v>
+      </c>
+    </row>
+    <row r="4850">
+      <c r="A4850" s="1" t="n">
+        <v>4848</v>
+      </c>
+      <c r="B4850" t="inlineStr">
+        <is>
+          <t>[7, 7, -10]</t>
+        </is>
+      </c>
+      <c r="C4850" t="n">
+        <v>13.99589512804003</v>
+      </c>
+    </row>
+    <row r="4851">
+      <c r="A4851" s="1" t="n">
+        <v>4849</v>
+      </c>
+      <c r="B4851" t="inlineStr">
+        <is>
+          <t>[8, 7, -10]</t>
+        </is>
+      </c>
+      <c r="C4851" t="n">
+        <v>13.96230703235925</v>
+      </c>
+    </row>
+    <row r="4852">
+      <c r="A4852" s="1" t="n">
+        <v>4850</v>
+      </c>
+      <c r="B4852" t="inlineStr">
+        <is>
+          <t>[9, 7, -10]</t>
+        </is>
+      </c>
+      <c r="C4852" t="n">
+        <v>13.93650056781341</v>
+      </c>
+    </row>
+    <row r="4853">
+      <c r="A4853" s="1" t="n">
+        <v>4851</v>
+      </c>
+      <c r="B4853" t="inlineStr">
+        <is>
+          <t>[10, 7, -10]</t>
+        </is>
+      </c>
+      <c r="C4853" t="n">
+        <v>13.92830850025918</v>
+      </c>
+    </row>
+    <row r="4854">
+      <c r="A4854" s="1" t="n">
+        <v>4852</v>
+      </c>
+      <c r="B4854" t="inlineStr">
+        <is>
+          <t>[10, 3, -3]</t>
+        </is>
+      </c>
+      <c r="C4854" t="n">
+        <v>13.91665511658073</v>
+      </c>
+    </row>
+    <row r="4855">
+      <c r="A4855" s="1" t="n">
+        <v>4853</v>
+      </c>
+      <c r="B4855" t="inlineStr">
+        <is>
+          <t>[9, 3, -3]</t>
+        </is>
+      </c>
+      <c r="C4855" t="n">
+        <v>13.9106067048705</v>
+      </c>
+    </row>
+    <row r="4856">
+      <c r="A4856" s="1" t="n">
+        <v>4854</v>
+      </c>
+      <c r="B4856" t="inlineStr">
+        <is>
+          <t>[5, 5, -6]</t>
+        </is>
+      </c>
+      <c r="C4856" t="n">
+        <v>13.95793455948127</v>
+      </c>
+    </row>
+    <row r="4857">
+      <c r="A4857" s="1" t="n">
+        <v>4855</v>
+      </c>
+      <c r="B4857" t="inlineStr">
+        <is>
+          <t>[7, 4, -4]</t>
+        </is>
+      </c>
+      <c r="C4857" t="n">
+        <v>14.02578384996823</v>
+      </c>
+    </row>
+    <row r="4858">
+      <c r="A4858" s="1" t="n">
+        <v>4856</v>
+      </c>
+      <c r="B4858" t="inlineStr">
+        <is>
+          <t>[8, 4, -4]</t>
+        </is>
+      </c>
+      <c r="C4858" t="n">
+        <v>13.94670374093734</v>
+      </c>
+    </row>
+    <row r="4859">
+      <c r="A4859" s="1" t="n">
+        <v>4857</v>
+      </c>
+      <c r="B4859" t="inlineStr">
+        <is>
+          <t>[9, 4, -4]</t>
+        </is>
+      </c>
+      <c r="C4859" t="n">
+        <v>13.90242066182663</v>
+      </c>
+    </row>
+    <row r="4860">
+      <c r="A4860" s="1" t="n">
+        <v>4858</v>
+      </c>
+      <c r="B4860" t="inlineStr">
+        <is>
+          <t>[10, 4, -4]</t>
+        </is>
+      </c>
+      <c r="C4860" t="n">
+        <v>13.91254106410707</v>
+      </c>
+    </row>
+    <row r="4861">
+      <c r="A4861" s="1" t="n">
+        <v>4859</v>
+      </c>
+      <c r="B4861" t="inlineStr">
+        <is>
+          <t>[4, 6, -7]</t>
+        </is>
+      </c>
+      <c r="C4861" t="n">
+        <v>14.03020169483665</v>
+      </c>
+    </row>
+    <row r="4862">
+      <c r="A4862" s="1" t="n">
+        <v>4860</v>
+      </c>
+      <c r="B4862" t="inlineStr">
+        <is>
+          <t>[8, 3, -3]</t>
+        </is>
+      </c>
+      <c r="C4862" t="n">
+        <v>13.95071514617291</v>
+      </c>
+    </row>
+    <row r="4863">
+      <c r="A4863" s="1" t="n">
+        <v>4861</v>
+      </c>
+      <c r="B4863" t="inlineStr">
+        <is>
+          <t>[3, 5, -5]</t>
+        </is>
+      </c>
+      <c r="C4863" t="n">
+        <v>14.34404106056383</v>
+      </c>
+    </row>
+    <row r="4864">
+      <c r="A4864" s="1" t="n">
+        <v>4862</v>
+      </c>
+      <c r="B4864" t="inlineStr">
+        <is>
+          <t>[4, 5, -5]</t>
+        </is>
+      </c>
+      <c r="C4864" t="n">
+        <v>14.06811448483414</v>
+      </c>
+    </row>
+    <row r="4865">
+      <c r="A4865" s="1" t="n">
+        <v>4863</v>
+      </c>
+      <c r="B4865" t="inlineStr">
+        <is>
+          <t>[5, 5, -5]</t>
+        </is>
+      </c>
+      <c r="C4865" t="n">
+        <v>13.9565506996864</v>
+      </c>
+    </row>
+    <row r="4866">
+      <c r="A4866" s="1" t="n">
+        <v>4864</v>
+      </c>
+      <c r="B4866" t="inlineStr">
+        <is>
+          <t>[6, 5, -5]</t>
+        </is>
+      </c>
+      <c r="C4866" t="n">
+        <v>14.03550825181737</v>
+      </c>
+    </row>
+    <row r="4867">
+      <c r="A4867" s="1" t="n">
+        <v>4865</v>
+      </c>
+      <c r="B4867" t="inlineStr">
+        <is>
+          <t>[7, 5, -5]</t>
+        </is>
+      </c>
+      <c r="C4867" t="n">
+        <v>14.0166034630625</v>
+      </c>
+    </row>
+    <row r="4868">
+      <c r="A4868" s="1" t="n">
+        <v>4866</v>
+      </c>
+      <c r="B4868" t="inlineStr">
+        <is>
+          <t>[8, 5, -5]</t>
+        </is>
+      </c>
+      <c r="C4868" t="n">
+        <v>13.94917129159791</v>
+      </c>
+    </row>
+    <row r="4869">
+      <c r="A4869" s="1" t="n">
+        <v>4867</v>
+      </c>
+      <c r="B4869" t="inlineStr">
+        <is>
+          <t>[9, 5, -5]</t>
+        </is>
+      </c>
+      <c r="C4869" t="n">
+        <v>13.90243756486538</v>
+      </c>
+    </row>
+    <row r="4870">
+      <c r="A4870" s="1" t="n">
+        <v>4868</v>
+      </c>
+      <c r="B4870" t="inlineStr">
+        <is>
+          <t>[10, 5, -5]</t>
+        </is>
+      </c>
+      <c r="C4870" t="n">
+        <v>13.90986007042025</v>
+      </c>
+    </row>
+    <row r="4871">
+      <c r="A4871" s="1" t="n">
+        <v>4869</v>
+      </c>
+      <c r="B4871" t="inlineStr">
+        <is>
+          <t>[1, 8, -10]</t>
+        </is>
+      </c>
+      <c r="C4871" t="n">
+        <v>15.13345083422618</v>
+      </c>
+    </row>
+    <row r="4872">
+      <c r="A4872" s="1" t="n">
+        <v>4870</v>
+      </c>
+      <c r="B4872" t="inlineStr">
+        <is>
+          <t>[2, 8, -10]</t>
+        </is>
+      </c>
+      <c r="C4872" t="n">
+        <v>14.66232408713203</v>
+      </c>
+    </row>
+    <row r="4873">
+      <c r="A4873" s="1" t="n">
+        <v>4871</v>
+      </c>
+      <c r="B4873" t="inlineStr">
+        <is>
+          <t>[0, 8, -10]</t>
+        </is>
+      </c>
+      <c r="C4873" t="n">
+        <v>15.278366380837</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>